<commit_message>
mikel@LAPTOP-73NPQ876 MINGW64 ~ $ cd D:Documents_progprog_custeclipse-workspace
mikel@LAPTOP-73NPQ876 MINGW64 /d/Documents/_prog/prog_cust/eclipse-workspace (master)
$ git add -A

mikel@LAPTOP-73NPQ876 MINGW64 /d/Documents/_prog/prog_cust/eclipse-workspace (master)
$ git commit -m
</commit_message>
<xml_diff>
--- a/graph_expr/output/goodcol_outputs/am_lb3_small_1query__ansgrBYVIEWS_newcols- faster 2.xlsx
+++ b/graph_expr/output/goodcol_outputs/am_lb3_small_1query__ansgrBYVIEWS_newcols- faster 2.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="mikel"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -14,10 +14,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1619543026" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1619543026" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1619543026"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1619543026"/>
+      <pm:revision xmlns:pm="smNativeData" day="1619559961" val="982" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1619559961" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1619559961"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1619559961"/>
     </ext>
   </extLst>
 </workbook>
@@ -183,7 +183,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619543026" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619559961" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -198,7 +198,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619543026" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619559961" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="240" lang="default"/>
             <pm:ea face="SimSun" sz="240" lang="default"/>
@@ -213,7 +213,7 @@
       <sz val="12"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619543026" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619559961" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="240" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -246,7 +246,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619543026"/>
+          <pm:border xmlns:pm="smNativeData" id="1619559961"/>
         </ext>
       </extLst>
     </border>
@@ -270,7 +270,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1619543026" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1619559961" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="L7" sqref="A7:L7"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -876,7 +876,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1619543026" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619559961" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -885,16 +885,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1619543026" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1619543026" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1619543026" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1619543026" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1619559961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619559961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1619559961" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1619559961" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619543026" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619559961" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -907,13 +907,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView view="normal" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.80"/>
   <cols>
-    <col min="1" max="16384" width="10.000000" style="3"/>
+    <col min="1" max="7" width="10.000000" style="3"/>
+    <col min="8" max="8" width="13.819820" customWidth="1" style="3"/>
+    <col min="9" max="9" width="14.828829" customWidth="1" style="3"/>
+    <col min="10" max="16384" width="10.000000" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384">
@@ -1066,7 +1069,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1619543026" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619559961" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1075,16 +1078,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1619543026" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1619543026" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1619543026" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1619543026" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1619559961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619559961" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1619559961" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1619559961" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619543026" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619559961" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>